<commit_message>
VideoAnalysis Protocols and Upload to google drive
</commit_message>
<xml_diff>
--- a/URUVS/Datasheets/Example_RecordingData.xlsx
+++ b/URUVS/Datasheets/Example_RecordingData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophi\Documents\GitHub\TanakekeProject\URUVS\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8800E01E-A690-4129-8595-D1CF9CFCAC9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC87B509-9188-4602-A748-D2D4DFBF71FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
+    <sheet name="MetaData" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>DATE</t>
   </si>
@@ -246,6 +247,81 @@
   </si>
   <si>
     <t>T1_UNIDGUPPY</t>
+  </si>
+  <si>
+    <t>Format: dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>TOMPOTANA OR LANTAMPEO</t>
+  </si>
+  <si>
+    <t>L/D/E</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>Number of deployment of the day</t>
+  </si>
+  <si>
+    <t>From field Notebook</t>
+  </si>
+  <si>
+    <t>From Field Notebook</t>
+  </si>
+  <si>
+    <t>In DD. Only if site has changed</t>
+  </si>
+  <si>
+    <t>Total number of files made with each recording</t>
+  </si>
+  <si>
+    <t>See field methods</t>
+  </si>
+  <si>
+    <t>From Fishing Points</t>
+  </si>
+  <si>
+    <t>Total time of each file</t>
+  </si>
+  <si>
+    <t>Time UNUSED from beginning file</t>
+  </si>
+  <si>
+    <t>Time UNUSED from end file</t>
+  </si>
+  <si>
+    <t>% of screen taken up by vegitation</t>
+  </si>
+  <si>
+    <t>From calib stick</t>
+  </si>
+  <si>
+    <t>Total number fish species found</t>
+  </si>
+  <si>
+    <t>MAXN FOR EACH FISH</t>
+  </si>
+  <si>
+    <t>TIME 1ST. NOTE: must add on time of previous files if t1 was in F2 or F3</t>
+  </si>
+  <si>
+    <t>MAXN_FISHNAME</t>
+  </si>
+  <si>
+    <t>TIME_1STFISHNAME</t>
+  </si>
+  <si>
+    <t>T1_FISHNAME</t>
+  </si>
+  <si>
+    <t>From Field (cm)</t>
+  </si>
+  <si>
+    <t>Estimated from field NB</t>
+  </si>
+  <si>
+    <t>From observation</t>
   </si>
 </sst>
 </file>
@@ -443,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -490,6 +566,60 @@
     <xf numFmtId="21" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,10 +902,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF2D75B-3330-44BB-BF8B-27BF0F133624}">
   <dimension ref="A1:BT20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BB1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="BO14" sqref="BO14"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3269,4 +3399,1111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C275047-2B6F-478B-B578-4E8B665EBECB}">
+  <dimension ref="A1:AJ20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI1" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ1" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="63" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="48"/>
+      <c r="G2" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="54">
+        <f>SUM(U2:W2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" s="54" t="e">
+        <f>X2-Y2-Z2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB2" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC2" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF2" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG2" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH2" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI2" s="61" t="e">
+        <f>IF(AG2=0,"NA",AH2-$Y2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ2" s="62"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21">
+        <f t="shared" ref="X3:X20" si="0">SUM(U3:W3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21">
+        <f t="shared" ref="AA3:AA20" si="1">X3-Y3-Z3</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="35" t="str">
+        <f t="shared" ref="AI3:AI20" si="2">IF(AG3=0,"NA",AH3-$Y3)</f>
+        <v>NA</v>
+      </c>
+      <c r="AJ3" s="38"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="32"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ4" s="38"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="32"/>
+      <c r="AG5" s="33"/>
+      <c r="AH5" s="36"/>
+      <c r="AI5" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ5" s="38"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="31"/>
+      <c r="AF6" s="32"/>
+      <c r="AG6" s="33"/>
+      <c r="AH6" s="36"/>
+      <c r="AI6" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ6" s="38"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="32"/>
+      <c r="AG7" s="33"/>
+      <c r="AH7" s="36"/>
+      <c r="AI7" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ7" s="38"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="33"/>
+      <c r="AH8" s="36"/>
+      <c r="AI8" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ8" s="38"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="36"/>
+      <c r="AI9" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ9" s="38"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="36"/>
+      <c r="AI10" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ10" s="38"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="32"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="36"/>
+      <c r="AI11" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ11" s="38"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="33"/>
+      <c r="AH12" s="36"/>
+      <c r="AI12" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ12" s="38"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="22"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="32"/>
+      <c r="AG13" s="33"/>
+      <c r="AH13" s="36"/>
+      <c r="AI13" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ13" s="38"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="33"/>
+      <c r="AH14" s="34"/>
+      <c r="AI14" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ14" s="38"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="32"/>
+      <c r="AG15" s="33"/>
+      <c r="AH15" s="34"/>
+      <c r="AI15" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ15" s="38"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="32"/>
+      <c r="AG16" s="33"/>
+      <c r="AH16" s="36"/>
+      <c r="AI16" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ16" s="38"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="21"/>
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="32"/>
+      <c r="AG17" s="33"/>
+      <c r="AH17" s="36"/>
+      <c r="AI17" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ17" s="38"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="32"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="36"/>
+      <c r="AI18" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ18" s="38"/>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="31"/>
+      <c r="AF19" s="32"/>
+      <c r="AG19" s="33"/>
+      <c r="AH19" s="36"/>
+      <c r="AI19" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ19" s="38"/>
+    </row>
+    <row r="20" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+      <c r="AD20" s="27"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="40"/>
+      <c r="AG20" s="41"/>
+      <c r="AH20" s="43"/>
+      <c r="AI20" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="AJ20" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>